<commit_message>
Dataset for data profiling and preprocessing
</commit_message>
<xml_diff>
--- a/StrategicDataManagementOrderData.xlsx
+++ b/StrategicDataManagementOrderData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WorknehYA\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WorknehYA\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F78D132-A7AC-42D6-B1E0-812376DDCD4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3A5F3D-638D-4211-8948-BE03F8147232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{EFFEC85E-F02C-7C4A-8D53-70B811AD1DE7}"/>
+    <workbookView xWindow="0" yWindow="610" windowWidth="19340" windowHeight="11390" xr2:uid="{EFFEC85E-F02C-7C4A-8D53-70B811AD1DE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -198,9 +198,6 @@
     <t>DSV492018573</t>
   </si>
   <si>
-    <t>DHS9812457031</t>
-  </si>
-  <si>
     <t>FDX6201948753</t>
   </si>
   <si>
@@ -213,27 +210,18 @@
     <t>UPS2859477021</t>
   </si>
   <si>
-    <t>DHS9518476204</t>
-  </si>
-  <si>
     <t>FDX4928175036</t>
   </si>
   <si>
     <t>UPS9732040032</t>
   </si>
   <si>
-    <t>DHS7841296507</t>
-  </si>
-  <si>
     <t>FDX2159083764</t>
   </si>
   <si>
     <t>UPS4837161188</t>
   </si>
   <si>
-    <t>DHS2849615709</t>
-  </si>
-  <si>
     <t>FDX9348207516</t>
   </si>
   <si>
@@ -246,9 +234,6 @@
     <t>UPS3482917062</t>
   </si>
   <si>
-    <t>DHS6401928751</t>
-  </si>
-  <si>
     <t>FDX8093156724</t>
   </si>
   <si>
@@ -258,12 +243,6 @@
     <t>UPS2839455010</t>
   </si>
   <si>
-    <t>DHS5419802364</t>
-  </si>
-  <si>
-    <t>DHS5928143</t>
-  </si>
-  <si>
     <t>FDX5728046139</t>
   </si>
   <si>
@@ -271,6 +250,27 @@
   </si>
   <si>
     <t>DSV7842093154</t>
+  </si>
+  <si>
+    <t>DHL9812457031</t>
+  </si>
+  <si>
+    <t>DHL9518476204</t>
+  </si>
+  <si>
+    <t>DHL7841296507</t>
+  </si>
+  <si>
+    <t>DHL2849615709</t>
+  </si>
+  <si>
+    <t>DHL6401928751</t>
+  </si>
+  <si>
+    <t>DHL5419802364</t>
+  </si>
+  <si>
+    <t>DHL5928143</t>
   </si>
 </sst>
 </file>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F21C4C-1F15-964C-98C1-85AE56BC84DD}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -859,7 +859,7 @@
         <v>22176</v>
       </c>
       <c r="J7" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -891,7 +891,7 @@
         <v>12048</v>
       </c>
       <c r="J8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -923,7 +923,7 @@
         <v>25463</v>
       </c>
       <c r="J9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -955,7 +955,7 @@
         <v>27518</v>
       </c>
       <c r="J10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -987,7 +987,7 @@
         <v>21174</v>
       </c>
       <c r="J11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1019,7 +1019,7 @@
         <v>8288</v>
       </c>
       <c r="J12" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -1051,7 +1051,7 @@
         <v>9181</v>
       </c>
       <c r="J13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -1115,7 +1115,7 @@
         <v>15688</v>
       </c>
       <c r="J15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -1147,7 +1147,7 @@
         <v>10590</v>
       </c>
       <c r="J16" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -1179,7 +1179,7 @@
         <v>21149</v>
       </c>
       <c r="J17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -1211,7 +1211,7 @@
         <v>14747</v>
       </c>
       <c r="J18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -1243,7 +1243,7 @@
         <v>20354</v>
       </c>
       <c r="J19" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -1275,7 +1275,7 @@
         <v>27192</v>
       </c>
       <c r="J20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -1307,7 +1307,7 @@
         <v>28388</v>
       </c>
       <c r="J21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -1339,7 +1339,7 @@
         <v>25164</v>
       </c>
       <c r="J22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
@@ -1371,7 +1371,7 @@
         <v>7830</v>
       </c>
       <c r="J23" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -1403,7 +1403,7 @@
         <v>31574</v>
       </c>
       <c r="J24" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
@@ -1435,7 +1435,7 @@
         <v>16361</v>
       </c>
       <c r="J25" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
@@ -1467,7 +1467,7 @@
         <v>13062</v>
       </c>
       <c r="J26" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
@@ -1499,7 +1499,7 @@
         <v>14872</v>
       </c>
       <c r="J27" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -1531,7 +1531,7 @@
         <v>14284</v>
       </c>
       <c r="J28" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -1563,7 +1563,7 @@
         <v>12980</v>
       </c>
       <c r="J29" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -1595,7 +1595,7 @@
         <v>20172</v>
       </c>
       <c r="J30" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
@@ -1627,7 +1627,7 @@
         <v>5166</v>
       </c>
       <c r="J31" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
@@ -1659,7 +1659,7 @@
         <v>28502</v>
       </c>
       <c r="J32" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
@@ -1691,7 +1691,7 @@
         <v>11866</v>
       </c>
       <c r="J33" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
@@ -1723,7 +1723,7 @@
         <v>15519</v>
       </c>
       <c r="J34" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>